<commit_message>
Updated on 16 th April
</commit_message>
<xml_diff>
--- a/DB and Documents/WASHB_DRAFT_MLHECommunity.xlsx
+++ b/DB and Documents/WASHB_DRAFT_MLHECommunity.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1539" uniqueCount="376">
   <si>
     <t>SLNo</t>
   </si>
@@ -2929,8 +2929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59:H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -5291,8 +5291,8 @@
         <v>161</v>
       </c>
       <c r="G63"/>
-      <c r="H63" t="s">
-        <v>177</v>
+      <c r="H63" s="140" t="s">
+        <v>184</v>
       </c>
       <c r="R63" s="140" t="s">
         <v>42</v>
@@ -5305,7 +5305,7 @@
       </c>
       <c r="V63" s="140" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('62', 'qRes1_7Other','frmtext', 'tblMainQues','7.mv¶vrKviPvwj‡q †h‡Z Pvqwb(কারণ উল্লেখ করুন)','7.Refused to continue the interview (mention the reason)','','qDate1Next','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('62', 'qRes1_7Other','frmtext', 'tblMainQues','7.mv¶vrKviPvwj‡q †h‡Z Pvqwb(কারণ উল্লেখ করুন)','7.Refused to continue the interview (mention the reason)','','qStart1','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
     <row r="64" spans="1:22" s="140" customFormat="1" ht="31.5">
@@ -5513,8 +5513,8 @@
         <v>161</v>
       </c>
       <c r="G69"/>
-      <c r="H69" t="s">
-        <v>180</v>
+      <c r="H69" s="140" t="s">
+        <v>185</v>
       </c>
       <c r="R69" s="140" t="s">
         <v>42</v>
@@ -5527,7 +5527,7 @@
       </c>
       <c r="V69" s="140" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('68', 'qRes2_7Other','frmtext', 'tblMainQues','7.mv¶vrKviPvwj‡q †h‡Z Pvqwb(কারণ উল্লেখ করুন)','7.Refused to continue the interview (mention the reason)','','qDate2Next','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('68', 'qRes2_7Other','frmtext', 'tblMainQues','7.mv¶vrKviPvwj‡q †h‡Z Pvqwb(কারণ উল্লেখ করুন)','7.Refused to continue the interview (mention the reason)','','qStart2','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
     <row r="70" spans="1:22" s="140" customFormat="1" ht="31.5">
@@ -6166,8 +6166,8 @@
       <c r="B87" t="s">
         <v>198</v>
       </c>
-      <c r="C87" t="s">
-        <v>32</v>
+      <c r="C87" s="140" t="s">
+        <v>131</v>
       </c>
       <c r="D87" t="s">
         <v>45</v>
@@ -6193,7 +6193,7 @@
       <c r="U87" s="140"/>
       <c r="V87" s="140" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('86', 'qSup','frmnumeric', 'tblMainQues','সুপারভাইজর আইডি','SUPERVISOR ID','','qField','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('86', 'qSup','frmcombobox', 'tblMainQues','সুপারভাইজর আইডি','SUPERVISOR ID','','qField','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
     <row r="88" spans="1:22">
@@ -6203,8 +6203,8 @@
       <c r="B88" t="s">
         <v>199</v>
       </c>
-      <c r="C88" t="s">
-        <v>32</v>
+      <c r="C88" s="140" t="s">
+        <v>131</v>
       </c>
       <c r="D88" t="s">
         <v>45</v>
@@ -6230,7 +6230,7 @@
       <c r="U88" s="140"/>
       <c r="V88" s="140" t="str">
         <f t="shared" si="1"/>
-        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('87', 'qField','frmnumeric', 'tblMainQues','ফিল্ডএডিটর আইডি ','FIELD EDITOR ID','','END','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
+        <v>insert into tblQuestion (SLNo, Qvar,Formname, Tablename, Qdescbng,Qdesceng,QType ,Qnext1,Qnext2, Qnext3, Qnext4, Qchoice1eng,Qchoice2eng,Qchoice3eng,Qchoice1Bng,Qchoice2Bng,Qchoice3Bng,Qrange1,Qrange2,DataType) values ('87', 'qField','frmcombobox', 'tblMainQues','ফিল্ডএডিটর আইডি ','FIELD EDITOR ID','','END','','', '','','','','','','',NULL,NULL,'nvarchar');</v>
       </c>
     </row>
   </sheetData>
@@ -6243,8 +6243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1305"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="G244" sqref="G244"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -6325,7 +6325,7 @@
         <v>167</v>
       </c>
       <c r="G3" s="125" t="str">
-        <f t="shared" ref="G3:G28" si="0">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A3&amp;"','" &amp;B3&amp;"', '" &amp;D3&amp;"','" &amp;C3&amp;"','" &amp;E3&amp;"','"&amp;F3&amp;"');"</f>
+        <f t="shared" ref="G3:G66" si="0">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A3&amp;"','" &amp;B3&amp;"', '" &amp;D3&amp;"','" &amp;C3&amp;"','" &amp;E3&amp;"','"&amp;F3&amp;"');"</f>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('2','qVisit', 'Second visit','২য় ভিজিট','2','qDate2');</v>
       </c>
     </row>
@@ -6369,10 +6369,12 @@
       <c r="E5" s="131">
         <v>1</v>
       </c>
-      <c r="F5" s="131"/>
+      <c r="F5" s="140" t="s">
+        <v>184</v>
+      </c>
       <c r="G5" s="125" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('4','qRes1', '1.Complete ','1.m¤ú~Y©','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('4','qRes1', '1.Complete ','1.m¤ú~Y©','1','qStart1');</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="126" customFormat="1" ht="25.5">
@@ -6391,13 +6393,15 @@
       <c r="E6" s="131">
         <v>2</v>
       </c>
-      <c r="F6" s="136"/>
+      <c r="F6" s="140" t="s">
+        <v>184</v>
+      </c>
       <c r="G6" s="125" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('5','qRes1', '2.Refused','2.Am¤§Z','2','');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="126" customFormat="1" ht="38.25">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('5','qRes1', '2.Refused','2.Am¤§Z','2','qStart1');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="126" customFormat="1" ht="25.5">
       <c r="A7" s="38">
         <v>6</v>
       </c>
@@ -6437,13 +6441,15 @@
       <c r="E8" s="131">
         <v>4</v>
       </c>
-      <c r="F8" s="131"/>
+      <c r="F8" s="140" t="s">
+        <v>184</v>
+      </c>
       <c r="G8" s="125" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('7','qRes1', '4.Incomplete','4.Am¤c~Y© ','4','');</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="126" customFormat="1" ht="38.25">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('7','qRes1', '4.Incomplete','4.Am¤c~Y© ','4','qStart1');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="126" customFormat="1" ht="28.5">
       <c r="A9" s="38">
         <v>8</v>
       </c>
@@ -6459,13 +6465,15 @@
       <c r="E9" s="131">
         <v>5</v>
       </c>
-      <c r="F9" s="136"/>
+      <c r="F9" s="140" t="s">
+        <v>184</v>
+      </c>
       <c r="G9" s="125" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('8','qRes1', '5.Household destroyed/Nobody lives at the house','5.emZevoxaŸsmcÖvß/Lvwj','5','');</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="126" customFormat="1" ht="38.25">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('8','qRes1', '5.Household destroyed/Nobody lives at the house','5.emZevoxaŸsmcÖvß/Lvwj','5','qStart1');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="126" customFormat="1" ht="25.5">
       <c r="A10" s="38">
         <v>9</v>
       </c>
@@ -6487,7 +6495,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('9','qRes1', '6.Respondent absent','6. DËi`vZv Abycw¯’Z','6','');</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="126" customFormat="1" ht="51">
+    <row r="11" spans="1:7" s="126" customFormat="1" ht="31.5">
       <c r="A11" s="38">
         <v>10</v>
       </c>
@@ -6511,7 +6519,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('10','qRes1', '7.Refused to continue the interview (mention the reason)','7.mv¶vrKviPvwj‡q †h‡Z Pvqwb(কারণ উল্লেখ করুন)','7','qRes1_7Other');</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="126" customFormat="1" ht="38.25">
+    <row r="12" spans="1:7" s="126" customFormat="1" ht="25.5">
       <c r="A12" s="38">
         <v>11</v>
       </c>
@@ -6551,10 +6559,12 @@
       <c r="E13" s="131">
         <v>1</v>
       </c>
-      <c r="F13" s="131"/>
+      <c r="F13" s="140" t="s">
+        <v>185</v>
+      </c>
       <c r="G13" s="125" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('12','qRes2', '1.Complete ','1.m¤ú~Y©','1','');</v>
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('12','qRes2', '1.Complete ','1.m¤ú~Y©','1','qStart2');</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="126" customFormat="1" ht="25.5">
@@ -6573,13 +6583,15 @@
       <c r="E14" s="131">
         <v>2</v>
       </c>
-      <c r="F14" s="136"/>
+      <c r="F14" s="140" t="s">
+        <v>185</v>
+      </c>
       <c r="G14" s="125" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('13','qRes2', '2.Refused','2.Am¤§Z','2','');</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="126" customFormat="1" ht="38.25">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('13','qRes2', '2.Refused','2.Am¤§Z','2','qStart2');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="126" customFormat="1" ht="25.5">
       <c r="A15" s="38">
         <v>14</v>
       </c>
@@ -6619,13 +6631,15 @@
       <c r="E16" s="131">
         <v>4</v>
       </c>
-      <c r="F16" s="131"/>
+      <c r="F16" s="140" t="s">
+        <v>185</v>
+      </c>
       <c r="G16" s="125" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('15','qRes2', '4.Incomplete','4.Am¤c~Y© ','4','');</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="126" customFormat="1" ht="38.25">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('15','qRes2', '4.Incomplete','4.Am¤c~Y© ','4','qStart2');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="126" customFormat="1" ht="28.5">
       <c r="A17" s="38">
         <v>16</v>
       </c>
@@ -6647,7 +6661,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('16','qRes2', '5.Household destroyed/Nobody lives at the house','5.emZevoxaŸsmcÖvß/Lvwj','5','');</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="126" customFormat="1" ht="38.25">
+    <row r="18" spans="1:7" s="126" customFormat="1" ht="25.5">
       <c r="A18" s="38">
         <v>17</v>
       </c>
@@ -6669,7 +6683,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('17','qRes2', '6.Respondent absent','6. DËi`vZv Abycw¯’Z','6','');</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="126" customFormat="1" ht="51">
+    <row r="19" spans="1:7" s="126" customFormat="1" ht="28.5">
       <c r="A19" s="38">
         <v>18</v>
       </c>
@@ -6693,7 +6707,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('18','qRes2', '7.Refused to continue the interview (mention the reason)','7.mv¶vrKviPvwj‡q †h‡Z Pvqwb(কারণ উল্লেখ করুন)','7','qRes2_7Other');</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="126" customFormat="1" ht="38.25">
+    <row r="20" spans="1:7" s="126" customFormat="1" ht="25.5">
       <c r="A20" s="38">
         <v>19</v>
       </c>
@@ -6755,15 +6769,13 @@
       <c r="E22" s="131">
         <v>2</v>
       </c>
-      <c r="F22" s="136" t="s">
-        <v>200</v>
-      </c>
+      <c r="F22" s="136"/>
       <c r="G22" s="125" t="str">
         <f t="shared" si="0"/>
-        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('21','qRes3', '2.Refused','2.Am¤§Z','2','END');</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="126" customFormat="1" ht="38.25">
+        <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('21','qRes3', '2.Refused','2.Am¤§Z','2','');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="126" customFormat="1" ht="25.5">
       <c r="A23" s="38">
         <v>22</v>
       </c>
@@ -6809,7 +6821,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('23','qRes3', '4.Incomplete','4.Am¤c~Y© ','4','');</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="126" customFormat="1" ht="38.25">
+    <row r="25" spans="1:7" s="126" customFormat="1" ht="28.5">
       <c r="A25" s="38">
         <v>24</v>
       </c>
@@ -6831,7 +6843,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('24','qRes3', '5.Household destroyed/Nobody lives at the house','5.emZevoxaŸsmcÖvß/Lvwj','5','');</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="126" customFormat="1" ht="38.25">
+    <row r="26" spans="1:7" s="126" customFormat="1" ht="25.5">
       <c r="A26" s="38">
         <v>25</v>
       </c>
@@ -6853,7 +6865,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('25','qRes3', '6.Respondent absent','6. DËi`vZv Abycw¯’Z','6','');</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="126" customFormat="1" ht="51">
+    <row r="27" spans="1:7" s="126" customFormat="1" ht="28.5">
       <c r="A27" s="38">
         <v>26</v>
       </c>
@@ -6877,7 +6889,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('26','qRes3', '7.Refused to continue the interview (mention the reason)','7.mv¶vrKviPvwj‡q †h‡Z Pvqwb(কারণ উল্লেখ করুন)','7','qRes3_7Other');</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="126" customFormat="1" ht="38.25">
+    <row r="28" spans="1:7" s="126" customFormat="1" ht="25.5">
       <c r="A28" s="38">
         <v>27</v>
       </c>
@@ -6919,7 +6931,7 @@
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="125" t="str">
-        <f>"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A29&amp;"','" &amp;B29&amp;"', '" &amp;D29&amp;"','" &amp;C29&amp;"','" &amp;E29&amp;"','"&amp;F29&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('28','q103', '1.ISLAM ','1.Bmjvg','1','');</v>
       </c>
     </row>
@@ -6941,7 +6953,7 @@
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="125" t="str">
-        <f t="shared" ref="G30:G93" si="1">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A30&amp;"','" &amp;B30&amp;"', '" &amp;D30&amp;"','" &amp;C30&amp;"','" &amp;E30&amp;"','"&amp;F30&amp;"');"</f>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('29','q103', '2.HINDUISM ','2.wn›`y','2','');</v>
       </c>
     </row>
@@ -6962,7 +6974,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('30','q103', '3.BUDDHISM ','3.†eŠ×','3','');</v>
       </c>
     </row>
@@ -6984,11 +6996,11 @@
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('31','q103', '4.CHRISTIANITY ','4.wLª÷vb','4','');</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="11" customFormat="1" ht="38.25">
+    <row r="33" spans="1:7" s="11" customFormat="1" ht="25.5">
       <c r="A33" s="38">
         <v>32</v>
       </c>
@@ -7008,7 +7020,7 @@
         <v>212</v>
       </c>
       <c r="G33" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('32','q103', '5.OTHER (Specify) ','5.Ab¨vb¨(wbw`©ó K‡i ejyb) ','5','q103Other');</v>
       </c>
     </row>
@@ -7029,7 +7041,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('33','q104', '1.Can read only','1.ïay co‡Z cv‡i','1','');</v>
       </c>
     </row>
@@ -7051,11 +7063,11 @@
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('34','q104', '2.Can write only','2.ïay wjL‡Z cv‡i','2','');</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="11" customFormat="1" ht="38.25">
+    <row r="36" spans="1:7" s="11" customFormat="1" ht="25.5">
       <c r="A36" s="38">
         <v>35</v>
       </c>
@@ -7073,7 +7085,7 @@
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('35','q104', '3.Can read and write','3.wjL‡Z I co‡Z cv‡i','3','');</v>
       </c>
     </row>
@@ -7094,7 +7106,7 @@
         <v>4</v>
       </c>
       <c r="G37" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('36','q104', '4.NONE','4.†KvbwUB cv‡ibv','4','');</v>
       </c>
     </row>
@@ -7115,7 +7127,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('37','q105', '1.YES, SCHOOL','1.nu¨v, ¯‹z‡j','1','');</v>
       </c>
     </row>
@@ -7136,7 +7148,7 @@
         <v>2</v>
       </c>
       <c r="G39" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('38','q105', '2.YES, MADRASHA','2.nu¨v, gv`ªvmv','2','');</v>
       </c>
     </row>
@@ -7158,7 +7170,7 @@
       </c>
       <c r="F40" s="10"/>
       <c r="G40" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('39','q105', '3.YES, BOTH','3.nu¨v, Dfq','3','');</v>
       </c>
     </row>
@@ -7182,11 +7194,11 @@
         <v>216</v>
       </c>
       <c r="G41" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('40','q105', '4.NO','4.bv','4','q107');</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="28" customFormat="1" ht="38.25">
+    <row r="42" spans="1:7" s="28" customFormat="1" ht="25.5">
       <c r="A42" s="38">
         <v>41</v>
       </c>
@@ -7206,7 +7218,7 @@
         <v>235</v>
       </c>
       <c r="G42" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('41','q105', '6.OTHERS (SPECIFY)','6.Ab¨vb¨ (wbw`©ó Kiæb)','6','q105Other');</v>
       </c>
     </row>
@@ -7227,7 +7239,7 @@
         <v>1</v>
       </c>
       <c r="G43" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('42','q107', '1.AGRICULTURE ','1.K…wlKvR','1','');</v>
       </c>
     </row>
@@ -7249,7 +7261,7 @@
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('43','q107', '2.RICKSHOW PULLER','2.wi·vIqvjv','2','');</v>
       </c>
     </row>
@@ -7271,11 +7283,11 @@
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('44','q107', '3.MECHANIC','3.†gKvwbK','3','');</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="11" customFormat="1" ht="38.25">
+    <row r="46" spans="1:7" s="11" customFormat="1" ht="25.5">
       <c r="A46" s="38">
         <v>45</v>
       </c>
@@ -7292,7 +7304,7 @@
         <v>4</v>
       </c>
       <c r="G46" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('45','q107', '4.BUS/TRUCK DRIVER','4.evm/ UªvK WªvBfvi','4','');</v>
       </c>
     </row>
@@ -7313,7 +7325,7 @@
         <v>5</v>
       </c>
       <c r="G47" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('46','q107', '5.CNG DRIVER','5.wmGbwR WªvBfvi','5','');</v>
       </c>
     </row>
@@ -7334,7 +7346,7 @@
         <v>6</v>
       </c>
       <c r="G48" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('47','q107', '6.SHOP KEEPER','6.†`vKvb`vi','6','');</v>
       </c>
     </row>
@@ -7356,11 +7368,11 @@
       </c>
       <c r="F49" s="10"/>
       <c r="G49" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('48','q107', '7.HANDICRAFTS','7.KzwUi wkí','7','');</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="11" customFormat="1" ht="38.25">
+    <row r="50" spans="1:7" s="11" customFormat="1" ht="25.5">
       <c r="A50" s="38">
         <v>49</v>
       </c>
@@ -7377,7 +7389,7 @@
         <v>8</v>
       </c>
       <c r="G50" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('49','q107', '8.SKILLED LABOUR','8.`¶ kªwgK (Kvgvi, Kzgvi, QyZvi, `wR©, gywP)','8','');</v>
       </c>
     </row>
@@ -7398,7 +7410,7 @@
         <v>9</v>
       </c>
       <c r="G51" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('50','q107', '9.VENDOR','9.†dwiIqvjv/ nKvi / ‡fÛvi','9','');</v>
       </c>
     </row>
@@ -7420,11 +7432,11 @@
       </c>
       <c r="F52" s="10"/>
       <c r="G52" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('51','q107', '10.DAILY LABOUR','10.w`bgRyi','10','');</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="11" customFormat="1" ht="38.25">
+    <row r="53" spans="1:7" s="11" customFormat="1" ht="25.5">
       <c r="A53" s="38">
         <v>52</v>
       </c>
@@ -7442,7 +7454,7 @@
       </c>
       <c r="F53" s="10"/>
       <c r="G53" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('52','q107', '11.BIUSNESS (small)','11.‡QvU e¨emv','11','');</v>
       </c>
     </row>
@@ -7463,11 +7475,11 @@
         <v>12</v>
       </c>
       <c r="G54" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('53','q107', '12.BIUSNESS (big)','12.eo e¨emv','12','');</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="11" customFormat="1" ht="38.25">
+    <row r="55" spans="1:7" s="11" customFormat="1" ht="25.5">
       <c r="A55" s="38">
         <v>54</v>
       </c>
@@ -7484,11 +7496,11 @@
         <v>13</v>
       </c>
       <c r="G55" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('54','q107', '13.GOVT. SERVICE','13.miKvwi PvKzwi','13','');</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="38.25">
+    <row r="56" spans="1:7" ht="25.5">
       <c r="A56" s="38">
         <v>55</v>
       </c>
@@ -7505,7 +7517,7 @@
         <v>14</v>
       </c>
       <c r="G56" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('55','q107', '14.PRIVATE SERVICE','14.†emiKvwi PvKzwi','14','');</v>
       </c>
     </row>
@@ -7526,11 +7538,11 @@
         <v>15</v>
       </c>
       <c r="G57" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('56','q107', '15.UNEMPLOYED','15.†eKvi','15','');</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="38.25">
+    <row r="58" spans="1:7" ht="25.5">
       <c r="A58" s="38">
         <v>57</v>
       </c>
@@ -7547,11 +7559,11 @@
         <v>16</v>
       </c>
       <c r="G58" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('57','q107', '16.GAEMENT WORKER','16.Mv‡g©›Um Kg©x','16','');</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="38.25">
+    <row r="59" spans="1:7" ht="25.5">
       <c r="A59" s="38">
         <v>58</v>
       </c>
@@ -7571,7 +7583,7 @@
         <v>217</v>
       </c>
       <c r="G59" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('58','q107', '96.OTHERS (SPECIFY)','96.Ab¨vb¨ (wbw`©ó Kiæb)','96','q107Other');</v>
       </c>
     </row>
@@ -7592,7 +7604,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('59','q201', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
@@ -7613,11 +7625,11 @@
         <v>2</v>
       </c>
       <c r="G61" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('60','q201', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="38.25">
+    <row r="62" spans="1:7" ht="25.5">
       <c r="A62" s="38">
         <v>61</v>
       </c>
@@ -7634,11 +7646,11 @@
         <v>8</v>
       </c>
       <c r="G62" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('61','q201', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="38.25">
+    <row r="63" spans="1:7" ht="25.5">
       <c r="A63" s="38">
         <v>62</v>
       </c>
@@ -7655,7 +7667,7 @@
         <v>9</v>
       </c>
       <c r="G63" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('62','q201', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -7676,7 +7688,7 @@
         <v>1</v>
       </c>
       <c r="G64" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('63','q202', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
@@ -7697,11 +7709,11 @@
         <v>2</v>
       </c>
       <c r="G65" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('64','q202', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="38.25">
+    <row r="66" spans="1:7" ht="25.5">
       <c r="A66" s="38">
         <v>65</v>
       </c>
@@ -7718,11 +7730,11 @@
         <v>8</v>
       </c>
       <c r="G66" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('65','q202', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="38.25">
+    <row r="67" spans="1:7" ht="25.5">
       <c r="A67" s="38">
         <v>66</v>
       </c>
@@ -7739,7 +7751,7 @@
         <v>9</v>
       </c>
       <c r="G67" s="125" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G67:G130" si="1">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A67&amp;"','" &amp;B67&amp;"', '" &amp;D67&amp;"','" &amp;C67&amp;"','" &amp;E67&amp;"','"&amp;F67&amp;"');"</f>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('66','q202', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -7786,7 +7798,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('68','q203', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="38.25">
+    <row r="70" spans="1:7" ht="25.5">
       <c r="A70" s="38">
         <v>69</v>
       </c>
@@ -7807,7 +7819,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('69','q203', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="38.25">
+    <row r="71" spans="1:7" ht="25.5">
       <c r="A71" s="38">
         <v>70</v>
       </c>
@@ -7870,7 +7882,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('72','q204', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="38.25">
+    <row r="74" spans="1:7" ht="25.5">
       <c r="A74" s="38">
         <v>73</v>
       </c>
@@ -7891,7 +7903,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('73','q204', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="38.25">
+    <row r="75" spans="1:7" ht="25.5">
       <c r="A75" s="38">
         <v>74</v>
       </c>
@@ -7955,7 +7967,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('76','q205', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="38.25">
+    <row r="78" spans="1:7" ht="25.5">
       <c r="A78" s="38">
         <v>77</v>
       </c>
@@ -7976,7 +7988,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('77','q205', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="38.25">
+    <row r="79" spans="1:7" ht="25.5">
       <c r="A79" s="38">
         <v>78</v>
       </c>
@@ -8039,7 +8051,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('80','q206', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="38.25">
+    <row r="82" spans="1:7" ht="25.5">
       <c r="A82" s="38">
         <v>81</v>
       </c>
@@ -8060,7 +8072,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('81','q206', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="38.25">
+    <row r="83" spans="1:7" ht="25.5">
       <c r="A83" s="38">
         <v>82</v>
       </c>
@@ -8123,7 +8135,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('84','q207', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="38.25">
+    <row r="86" spans="1:7" ht="25.5">
       <c r="A86" s="38">
         <v>85</v>
       </c>
@@ -8144,7 +8156,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('85','q207', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="38.25">
+    <row r="87" spans="1:7" ht="25.5">
       <c r="A87" s="38">
         <v>86</v>
       </c>
@@ -8207,7 +8219,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('88','q208', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="38.25">
+    <row r="90" spans="1:7" ht="25.5">
       <c r="A90" s="38">
         <v>89</v>
       </c>
@@ -8228,7 +8240,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('89','q208', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="38.25">
+    <row r="91" spans="1:7" ht="25.5">
       <c r="A91" s="38">
         <v>90</v>
       </c>
@@ -8291,7 +8303,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('92','q209', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="38.25">
+    <row r="94" spans="1:7" ht="25.5">
       <c r="A94" s="38">
         <v>93</v>
       </c>
@@ -8309,11 +8321,11 @@
       </c>
       <c r="F94" s="4"/>
       <c r="G94" s="125" t="str">
-        <f t="shared" ref="G94:G157" si="2">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A94&amp;"','" &amp;B94&amp;"', '" &amp;D94&amp;"','" &amp;C94&amp;"','" &amp;E94&amp;"','"&amp;F94&amp;"');"</f>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('93','q209', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="38.25">
+    <row r="95" spans="1:7" ht="25.5">
       <c r="A95" s="38">
         <v>94</v>
       </c>
@@ -8330,7 +8342,7 @@
         <v>9</v>
       </c>
       <c r="G95" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('94','q209', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -8351,7 +8363,7 @@
         <v>1</v>
       </c>
       <c r="G96" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('95','q210', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
@@ -8372,11 +8384,11 @@
         <v>2</v>
       </c>
       <c r="G97" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('96','q210', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="38.25">
+    <row r="98" spans="1:8" ht="25.5">
       <c r="A98" s="38">
         <v>97</v>
       </c>
@@ -8393,11 +8405,11 @@
         <v>8</v>
       </c>
       <c r="G98" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('97','q210', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="38.25">
+    <row r="99" spans="1:8" ht="25.5">
       <c r="A99" s="38">
         <v>98</v>
       </c>
@@ -8414,7 +8426,7 @@
         <v>9</v>
       </c>
       <c r="G99" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('98','q210', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -8435,7 +8447,7 @@
         <v>1</v>
       </c>
       <c r="G100" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('99','q211', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
@@ -8456,11 +8468,11 @@
         <v>2</v>
       </c>
       <c r="G101" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('100','q211', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="38.25">
+    <row r="102" spans="1:8" ht="25.5">
       <c r="A102" s="38">
         <v>101</v>
       </c>
@@ -8478,11 +8490,11 @@
       </c>
       <c r="F102" s="3"/>
       <c r="G102" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('101','q211', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="38.25">
+    <row r="103" spans="1:8" ht="25.5">
       <c r="A103" s="38">
         <v>102</v>
       </c>
@@ -8499,7 +8511,7 @@
         <v>9</v>
       </c>
       <c r="G103" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('102','q211', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -8520,7 +8532,7 @@
         <v>1</v>
       </c>
       <c r="G104" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('103','q212', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
@@ -8541,11 +8553,11 @@
         <v>2</v>
       </c>
       <c r="G105" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('104','q212', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="38.25">
+    <row r="106" spans="1:8" ht="25.5">
       <c r="A106" s="38">
         <v>105</v>
       </c>
@@ -8562,11 +8574,11 @@
         <v>8</v>
       </c>
       <c r="G106" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('105','q212', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="38.25">
+    <row r="107" spans="1:8" ht="25.5">
       <c r="A107" s="38">
         <v>106</v>
       </c>
@@ -8583,7 +8595,7 @@
         <v>9</v>
       </c>
       <c r="G107" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('106','q212', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -8604,7 +8616,7 @@
         <v>1</v>
       </c>
       <c r="G108" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('107','q213', '1.AGREE','1.GKgZ','1','');</v>
       </c>
       <c r="H108" s="6"/>
@@ -8627,12 +8639,12 @@
       </c>
       <c r="F109" s="6"/>
       <c r="G109" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('108','q213', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
       <c r="H109" s="6"/>
     </row>
-    <row r="110" spans="1:8" s="7" customFormat="1" ht="38.25">
+    <row r="110" spans="1:8" s="7" customFormat="1" ht="25.5">
       <c r="A110" s="38">
         <v>109</v>
       </c>
@@ -8649,12 +8661,12 @@
         <v>8</v>
       </c>
       <c r="G110" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('109','q213', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
       <c r="H110" s="6"/>
     </row>
-    <row r="111" spans="1:8" ht="38.25">
+    <row r="111" spans="1:8" ht="25.5">
       <c r="A111" s="38">
         <v>110</v>
       </c>
@@ -8671,7 +8683,7 @@
         <v>9</v>
       </c>
       <c r="G111" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('110','q213', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -8692,7 +8704,7 @@
         <v>1</v>
       </c>
       <c r="G112" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('111','q214', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
@@ -8713,11 +8725,11 @@
         <v>2</v>
       </c>
       <c r="G113" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('112','q214', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="38.25">
+    <row r="114" spans="1:7" ht="25.5">
       <c r="A114" s="38">
         <v>113</v>
       </c>
@@ -8734,11 +8746,11 @@
         <v>8</v>
       </c>
       <c r="G114" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('113','q214', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="38.25">
+    <row r="115" spans="1:7" ht="25.5">
       <c r="A115" s="38">
         <v>114</v>
       </c>
@@ -8755,7 +8767,7 @@
         <v>9</v>
       </c>
       <c r="G115" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('114','q214', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -8776,7 +8788,7 @@
         <v>1</v>
       </c>
       <c r="G116" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('115','q215', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
@@ -8797,11 +8809,11 @@
         <v>2</v>
       </c>
       <c r="G117" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('116','q215', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="118" spans="1:7" s="7" customFormat="1" ht="38.25">
+    <row r="118" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A118" s="38">
         <v>117</v>
       </c>
@@ -8818,11 +8830,11 @@
         <v>8</v>
       </c>
       <c r="G118" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('117','q215', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="119" spans="1:7" s="7" customFormat="1" ht="38.25">
+    <row r="119" spans="1:7" s="7" customFormat="1" ht="25.5">
       <c r="A119" s="38">
         <v>118</v>
       </c>
@@ -8839,7 +8851,7 @@
         <v>9</v>
       </c>
       <c r="G119" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('118','q215', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -8860,7 +8872,7 @@
         <v>1</v>
       </c>
       <c r="G120" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('119','q216', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
@@ -8881,11 +8893,11 @@
         <v>2</v>
       </c>
       <c r="G121" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('120','q216', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="38.25">
+    <row r="122" spans="1:7" ht="25.5">
       <c r="A122" s="38">
         <v>121</v>
       </c>
@@ -8903,11 +8915,11 @@
       </c>
       <c r="F122" s="3"/>
       <c r="G122" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('121','q216', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="38.25">
+    <row r="123" spans="1:7" ht="25.5">
       <c r="A123" s="38">
         <v>122</v>
       </c>
@@ -8925,7 +8937,7 @@
       </c>
       <c r="F123" s="3"/>
       <c r="G123" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('122','q216', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -8946,7 +8958,7 @@
         <v>1</v>
       </c>
       <c r="G124" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('123','q217', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
@@ -8967,11 +8979,11 @@
         <v>2</v>
       </c>
       <c r="G125" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('124','q217', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="38.25">
+    <row r="126" spans="1:7" ht="25.5">
       <c r="A126" s="38">
         <v>125</v>
       </c>
@@ -8988,11 +9000,11 @@
         <v>8</v>
       </c>
       <c r="G126" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('125','q217', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="38.25">
+    <row r="127" spans="1:7" ht="25.5">
       <c r="A127" s="38">
         <v>126</v>
       </c>
@@ -9010,7 +9022,7 @@
       </c>
       <c r="F127" s="3"/>
       <c r="G127" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('126','q217', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -9031,7 +9043,7 @@
         <v>1</v>
       </c>
       <c r="G128" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('127','q218', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
@@ -9052,11 +9064,11 @@
         <v>2</v>
       </c>
       <c r="G129" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('128','q218', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="38.25">
+    <row r="130" spans="1:7" ht="25.5">
       <c r="A130" s="38">
         <v>129</v>
       </c>
@@ -9073,11 +9085,11 @@
         <v>8</v>
       </c>
       <c r="G130" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('129','q218', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="38.25">
+    <row r="131" spans="1:7" ht="25.5">
       <c r="A131" s="38">
         <v>130</v>
       </c>
@@ -9094,7 +9106,7 @@
         <v>9</v>
       </c>
       <c r="G131" s="125" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="G131:G194" si="2">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A131&amp;"','" &amp;B131&amp;"', '" &amp;D131&amp;"','" &amp;C131&amp;"','" &amp;E131&amp;"','"&amp;F131&amp;"');"</f>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('130','q218', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -9140,7 +9152,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('132','q219', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="38.25">
+    <row r="134" spans="1:7" ht="25.5">
       <c r="A134" s="38">
         <v>133</v>
       </c>
@@ -9161,7 +9173,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('133','q219', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="38.25">
+    <row r="135" spans="1:7" ht="25.5">
       <c r="A135" s="38">
         <v>134</v>
       </c>
@@ -9225,7 +9237,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('136','q220', '2.DISAGREE','2.wØgZ','2','');</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="38.25">
+    <row r="138" spans="1:7" ht="25.5">
       <c r="A138" s="38">
         <v>137</v>
       </c>
@@ -9247,7 +9259,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('137','q220', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="38.25">
+    <row r="139" spans="1:7" ht="25.5">
       <c r="A139" s="38">
         <v>138</v>
       </c>
@@ -9289,7 +9301,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('139','q221', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="141" spans="1:7" s="115" customFormat="1" ht="38.25">
+    <row r="141" spans="1:7" s="115" customFormat="1" ht="25.5">
       <c r="A141" s="38">
         <v>140</v>
       </c>
@@ -9331,7 +9343,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('141','q221', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="38.25">
+    <row r="143" spans="1:7" ht="25.5">
       <c r="A143" s="38">
         <v>142</v>
       </c>
@@ -9352,7 +9364,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('142','q221', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="38.25">
+    <row r="144" spans="1:7" ht="25.5">
       <c r="A144" s="38">
         <v>143</v>
       </c>
@@ -9394,7 +9406,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('144','q222', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="38.25">
+    <row r="146" spans="1:7" ht="25.5">
       <c r="A146" s="38">
         <v>145</v>
       </c>
@@ -9436,7 +9448,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('146','q222', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="38.25">
+    <row r="148" spans="1:7" ht="25.5">
       <c r="A148" s="38">
         <v>147</v>
       </c>
@@ -9457,7 +9469,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('147','q222', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="38.25">
+    <row r="149" spans="1:7" ht="25.5">
       <c r="A149" s="38">
         <v>148</v>
       </c>
@@ -9499,7 +9511,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('149','q223', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="38.25">
+    <row r="151" spans="1:7" ht="25.5">
       <c r="A151" s="38">
         <v>150</v>
       </c>
@@ -9541,7 +9553,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('151','q223', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="38.25">
+    <row r="153" spans="1:7" ht="25.5">
       <c r="A153" s="38">
         <v>152</v>
       </c>
@@ -9562,7 +9574,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('152','q223', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="38.25">
+    <row r="154" spans="1:7" ht="25.5">
       <c r="A154" s="38">
         <v>153</v>
       </c>
@@ -9605,7 +9617,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('154','q224', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="38.25">
+    <row r="156" spans="1:7" ht="25.5">
       <c r="A156" s="38">
         <v>155</v>
       </c>
@@ -9647,7 +9659,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('156','q224', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="38.25">
+    <row r="158" spans="1:7" ht="25.5">
       <c r="A158" s="38">
         <v>157</v>
       </c>
@@ -9664,11 +9676,11 @@
         <v>8</v>
       </c>
       <c r="G158" s="125" t="str">
-        <f t="shared" ref="G158:G221" si="3">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A158&amp;"','" &amp;B158&amp;"', '" &amp;D158&amp;"','" &amp;C158&amp;"','" &amp;E158&amp;"','"&amp;F158&amp;"');"</f>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('157','q224', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="38.25">
+    <row r="159" spans="1:7" ht="25.5">
       <c r="A159" s="38">
         <v>158</v>
       </c>
@@ -9685,7 +9697,7 @@
         <v>9</v>
       </c>
       <c r="G159" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('158','q224', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -9706,11 +9718,11 @@
         <v>1</v>
       </c>
       <c r="G160" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('159','q225', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="38.25">
+    <row r="161" spans="1:7" ht="25.5">
       <c r="A161" s="38">
         <v>160</v>
       </c>
@@ -9727,7 +9739,7 @@
         <v>2</v>
       </c>
       <c r="G161" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('160','q225', '2.PARTIALLY AGREE','2.wKQzUv GKgZ','2','');</v>
       </c>
     </row>
@@ -9748,11 +9760,11 @@
         <v>3</v>
       </c>
       <c r="G162" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('161','q225', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="38.25">
+    <row r="163" spans="1:7" ht="25.5">
       <c r="A163" s="38">
         <v>162</v>
       </c>
@@ -9769,11 +9781,11 @@
         <v>8</v>
       </c>
       <c r="G163" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('162','q225', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="38.25">
+    <row r="164" spans="1:7" ht="25.5">
       <c r="A164" s="38">
         <v>163</v>
       </c>
@@ -9790,7 +9802,7 @@
         <v>9</v>
       </c>
       <c r="G164" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('163','q225', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -9811,11 +9823,11 @@
         <v>1</v>
       </c>
       <c r="G165" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('164','q226', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="38.25">
+    <row r="166" spans="1:7" ht="25.5">
       <c r="A166" s="38">
         <v>165</v>
       </c>
@@ -9832,7 +9844,7 @@
         <v>2</v>
       </c>
       <c r="G166" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('165','q226', '2.PARTIALLY AGREE','2.wKQzUv GKgZ','2','');</v>
       </c>
     </row>
@@ -9853,11 +9865,11 @@
         <v>3</v>
       </c>
       <c r="G167" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('166','q226', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="38.25">
+    <row r="168" spans="1:7" ht="25.5">
       <c r="A168" s="38">
         <v>167</v>
       </c>
@@ -9874,11 +9886,11 @@
         <v>8</v>
       </c>
       <c r="G168" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('167','q226', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="38.25">
+    <row r="169" spans="1:7" ht="25.5">
       <c r="A169" s="38">
         <v>168</v>
       </c>
@@ -9895,7 +9907,7 @@
         <v>9</v>
       </c>
       <c r="G169" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('168','q226', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -9916,11 +9928,11 @@
         <v>1</v>
       </c>
       <c r="G170" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('169','q227', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="38.25">
+    <row r="171" spans="1:7" ht="25.5">
       <c r="A171" s="38">
         <v>170</v>
       </c>
@@ -9937,7 +9949,7 @@
         <v>2</v>
       </c>
       <c r="G171" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('170','q227', '2.PARTIALLY AGREE','2.wKQzUv GKgZ','2','');</v>
       </c>
     </row>
@@ -9958,11 +9970,11 @@
         <v>3</v>
       </c>
       <c r="G172" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('171','q227', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="38.25">
+    <row r="173" spans="1:7" ht="25.5">
       <c r="A173" s="38">
         <v>172</v>
       </c>
@@ -9979,11 +9991,11 @@
         <v>8</v>
       </c>
       <c r="G173" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('172','q227', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="38.25">
+    <row r="174" spans="1:7" ht="25.5">
       <c r="A174" s="38">
         <v>173</v>
       </c>
@@ -10000,7 +10012,7 @@
         <v>9</v>
       </c>
       <c r="G174" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('173','q227', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -10021,11 +10033,11 @@
         <v>1</v>
       </c>
       <c r="G175" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('174','q228', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="38.25">
+    <row r="176" spans="1:7" ht="25.5">
       <c r="A176" s="38">
         <v>175</v>
       </c>
@@ -10042,7 +10054,7 @@
         <v>2</v>
       </c>
       <c r="G176" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('175','q228', '2.PARTIALLY AGREE','2.wKQzUv GKgZ','2','');</v>
       </c>
     </row>
@@ -10063,11 +10075,11 @@
         <v>3</v>
       </c>
       <c r="G177" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('176','q228', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="38.25">
+    <row r="178" spans="1:7" ht="25.5">
       <c r="A178" s="38">
         <v>177</v>
       </c>
@@ -10084,11 +10096,11 @@
         <v>8</v>
       </c>
       <c r="G178" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('177','q228', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="38.25">
+    <row r="179" spans="1:7" ht="25.5">
       <c r="A179" s="38">
         <v>178</v>
       </c>
@@ -10105,7 +10117,7 @@
         <v>9</v>
       </c>
       <c r="G179" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('178','q228', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -10126,11 +10138,11 @@
         <v>1</v>
       </c>
       <c r="G180" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('179','q229', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="38.25">
+    <row r="181" spans="1:7" ht="25.5">
       <c r="A181" s="38">
         <v>180</v>
       </c>
@@ -10147,7 +10159,7 @@
         <v>2</v>
       </c>
       <c r="G181" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('180','q229', '2.PARTIALLY AGREE','2.wKQzUv GKgZ','2','');</v>
       </c>
     </row>
@@ -10168,11 +10180,11 @@
         <v>3</v>
       </c>
       <c r="G182" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('181','q229', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="38.25">
+    <row r="183" spans="1:7" ht="25.5">
       <c r="A183" s="38">
         <v>182</v>
       </c>
@@ -10189,11 +10201,11 @@
         <v>8</v>
       </c>
       <c r="G183" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('182','q229', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="38.25">
+    <row r="184" spans="1:7" ht="25.5">
       <c r="A184" s="38">
         <v>183</v>
       </c>
@@ -10210,7 +10222,7 @@
         <v>9</v>
       </c>
       <c r="G184" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('183','q229', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -10231,11 +10243,11 @@
         <v>1</v>
       </c>
       <c r="G185" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('184','q230', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="38.25">
+    <row r="186" spans="1:7" ht="25.5">
       <c r="A186" s="38">
         <v>185</v>
       </c>
@@ -10252,7 +10264,7 @@
         <v>2</v>
       </c>
       <c r="G186" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('185','q230', '2.PARTIALLY AGREE','2.wKQzUv GKgZ','2','');</v>
       </c>
     </row>
@@ -10273,11 +10285,11 @@
         <v>3</v>
       </c>
       <c r="G187" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('186','q230', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="38.25">
+    <row r="188" spans="1:7" ht="25.5">
       <c r="A188" s="38">
         <v>187</v>
       </c>
@@ -10294,11 +10306,11 @@
         <v>8</v>
       </c>
       <c r="G188" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('187','q230', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="38.25">
+    <row r="189" spans="1:7" ht="25.5">
       <c r="A189" s="38">
         <v>188</v>
       </c>
@@ -10315,7 +10327,7 @@
         <v>9</v>
       </c>
       <c r="G189" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('188','q230', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -10336,11 +10348,11 @@
         <v>1</v>
       </c>
       <c r="G190" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('189','q231', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="38.25">
+    <row r="191" spans="1:7" ht="25.5">
       <c r="A191" s="38">
         <v>190</v>
       </c>
@@ -10357,7 +10369,7 @@
         <v>2</v>
       </c>
       <c r="G191" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('190','q231', '2.PARTIALLY AGREE','2.wKQzUv GKgZ','2','');</v>
       </c>
     </row>
@@ -10378,11 +10390,11 @@
         <v>3</v>
       </c>
       <c r="G192" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('191','q231', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="38.25">
+    <row r="193" spans="1:7" ht="25.5">
       <c r="A193" s="38">
         <v>192</v>
       </c>
@@ -10399,11 +10411,11 @@
         <v>8</v>
       </c>
       <c r="G193" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('192','q231', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="38.25">
+    <row r="194" spans="1:7" ht="25.5">
       <c r="A194" s="38">
         <v>193</v>
       </c>
@@ -10420,7 +10432,7 @@
         <v>9</v>
       </c>
       <c r="G194" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('193','q231', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -10441,11 +10453,11 @@
         <v>1</v>
       </c>
       <c r="G195" s="125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="G195:G236" si="3">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A195&amp;"','" &amp;B195&amp;"', '" &amp;D195&amp;"','" &amp;C195&amp;"','" &amp;E195&amp;"','"&amp;F195&amp;"');"</f>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('194','q232', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="196" spans="1:7" ht="38.25">
+    <row r="196" spans="1:7" ht="25.5">
       <c r="A196" s="38">
         <v>195</v>
       </c>
@@ -10487,7 +10499,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('196','q232', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="38.25">
+    <row r="198" spans="1:7" ht="25.5">
       <c r="A198" s="38">
         <v>197</v>
       </c>
@@ -10508,7 +10520,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('197','q232', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="199" spans="1:7" ht="38.25">
+    <row r="199" spans="1:7" ht="25.5">
       <c r="A199" s="38">
         <v>198</v>
       </c>
@@ -10551,7 +10563,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('199','q233', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="38.25">
+    <row r="201" spans="1:7" ht="25.5">
       <c r="A201" s="38">
         <v>200</v>
       </c>
@@ -10595,7 +10607,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('201','q233', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="203" spans="1:7" ht="38.25">
+    <row r="203" spans="1:7" ht="25.5">
       <c r="A203" s="38">
         <v>202</v>
       </c>
@@ -10617,7 +10629,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('202','q233', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="204" spans="1:7" ht="38.25">
+    <row r="204" spans="1:7" ht="25.5">
       <c r="A204" s="38">
         <v>203</v>
       </c>
@@ -10660,7 +10672,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('204','q234', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="206" spans="1:7" ht="38.25">
+    <row r="206" spans="1:7" ht="25.5">
       <c r="A206" s="38">
         <v>205</v>
       </c>
@@ -10703,7 +10715,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('206','q234', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="208" spans="1:7" ht="38.25">
+    <row r="208" spans="1:7" ht="25.5">
       <c r="A208" s="38">
         <v>207</v>
       </c>
@@ -10725,7 +10737,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('207','q234', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="209" spans="1:7" ht="38.25">
+    <row r="209" spans="1:7" ht="25.5">
       <c r="A209" s="38">
         <v>208</v>
       </c>
@@ -10767,7 +10779,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('209','q235', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="38.25">
+    <row r="211" spans="1:7" ht="25.5">
       <c r="A211" s="38">
         <v>210</v>
       </c>
@@ -10809,7 +10821,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('211','q235', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="38.25">
+    <row r="213" spans="1:7" ht="25.5">
       <c r="A213" s="38">
         <v>212</v>
       </c>
@@ -10830,7 +10842,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('212','q235', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="38.25">
+    <row r="214" spans="1:7" ht="25.5">
       <c r="A214" s="38">
         <v>213</v>
       </c>
@@ -10872,7 +10884,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('214','q236', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="38.25">
+    <row r="216" spans="1:7" ht="25.5">
       <c r="A216" s="38">
         <v>215</v>
       </c>
@@ -10914,7 +10926,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('216','q236', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="38.25">
+    <row r="218" spans="1:7" ht="25.5">
       <c r="A218" s="38">
         <v>217</v>
       </c>
@@ -10935,7 +10947,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('217','q236', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="219" spans="1:7" ht="38.25">
+    <row r="219" spans="1:7" ht="25.5">
       <c r="A219" s="38">
         <v>218</v>
       </c>
@@ -10977,7 +10989,7 @@
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('219','q237', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="221" spans="1:7" ht="38.25">
+    <row r="221" spans="1:7" ht="25.5">
       <c r="A221" s="38">
         <v>220</v>
       </c>
@@ -11015,11 +11027,11 @@
         <v>3</v>
       </c>
       <c r="G222" s="125" t="str">
-        <f t="shared" ref="G222:G236" si="4">"insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('" &amp;A222&amp;"','" &amp;B222&amp;"', '" &amp;D222&amp;"','" &amp;C222&amp;"','" &amp;E222&amp;"','"&amp;F222&amp;"');"</f>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('221','q237', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="38.25">
+    <row r="223" spans="1:7" ht="25.5">
       <c r="A223" s="38">
         <v>222</v>
       </c>
@@ -11036,11 +11048,11 @@
         <v>8</v>
       </c>
       <c r="G223" s="125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('222','q237', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="38.25">
+    <row r="224" spans="1:7" ht="25.5">
       <c r="A224" s="38">
         <v>223</v>
       </c>
@@ -11057,7 +11069,7 @@
         <v>9</v>
       </c>
       <c r="G224" s="125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('223','q237', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
@@ -11078,11 +11090,11 @@
         <v>1</v>
       </c>
       <c r="G225" s="125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('224','q238', '1.AGREE','1.GKgZ','1','');</v>
       </c>
     </row>
-    <row r="226" spans="1:7" ht="38.25">
+    <row r="226" spans="1:7" ht="25.5">
       <c r="A226" s="38">
         <v>225</v>
       </c>
@@ -11099,7 +11111,7 @@
         <v>2</v>
       </c>
       <c r="G226" s="125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('225','q238', '2.PARTIALLY AGREE','2.wKQzUv GKgZ','2','');</v>
       </c>
     </row>
@@ -11120,11 +11132,11 @@
         <v>3</v>
       </c>
       <c r="G227" s="125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('226','q238', '3.DISAGREE','3.GKgZ bq','3','');</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="38.25">
+    <row r="228" spans="1:7" ht="25.5">
       <c r="A228" s="38">
         <v>227</v>
       </c>
@@ -11141,11 +11153,11 @@
         <v>8</v>
       </c>
       <c r="G228" s="125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('227','q238', '8.DON’T KNOW/DON’T REMEMBER','8.Rvwbbv/g‡b ‡bB','8','');</v>
       </c>
     </row>
-    <row r="229" spans="1:7" ht="38.25">
+    <row r="229" spans="1:7" ht="25.5">
       <c r="A229" s="38">
         <v>228</v>
       </c>
@@ -11162,11 +11174,11 @@
         <v>9</v>
       </c>
       <c r="G229" s="125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('228','q238', '9.REFUSED/NO ANSWER','9.cÖZ¨vLvb Kiv/‡Kvb DËi bvB','9','');</v>
       </c>
     </row>
-    <row r="230" spans="1:7" ht="38.25">
+    <row r="230" spans="1:7" ht="25.5">
       <c r="A230" s="38">
         <v>229</v>
       </c>
@@ -11183,7 +11195,7 @@
         <v>0</v>
       </c>
       <c r="G230" s="125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('229','q239_4', 'd) He mistreats her','N.Zvi ¯^vgx Lvivc AvPib K‡i','0','');</v>
       </c>
     </row>
@@ -11204,11 +11216,11 @@
         <v>0</v>
       </c>
       <c r="G231" s="125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('230','q239_3', 'c) She is sick','M.¯¿x Amy¯’ _v‡K','0','');</v>
       </c>
     </row>
-    <row r="232" spans="1:7" ht="38.25">
+    <row r="232" spans="1:7" ht="25.5">
       <c r="A232" s="38">
         <v>231</v>
       </c>
@@ -11225,11 +11237,11 @@
         <v>0</v>
       </c>
       <c r="G232" s="125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('231','q239_2', 'b) He is drunk','L.Zvi ¯^vgx gvZvj Ae¯’vq _v‡K','0','');</v>
       </c>
     </row>
-    <row r="233" spans="1:7" ht="38.25">
+    <row r="233" spans="1:7" ht="25.5">
       <c r="A233" s="38">
         <v>232</v>
       </c>
@@ -11246,7 +11258,7 @@
         <v>0</v>
       </c>
       <c r="G233" s="125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('232','q239_1', 'a) She doesn’t want to','K.¯¿xi B”Qv bv _v‡K','0','');</v>
       </c>
     </row>
@@ -11267,7 +11279,7 @@
         <v>1</v>
       </c>
       <c r="G234" s="125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('233','q239_Options', '1.YES ','1.nu¨v','1','');</v>
       </c>
     </row>
@@ -11288,7 +11300,7 @@
         <v>2</v>
       </c>
       <c r="G235" s="125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('234','q239_Options', '2.NO','2.bv','2','');</v>
       </c>
     </row>
@@ -11309,7 +11321,7 @@
         <v>8</v>
       </c>
       <c r="G236" s="125" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>insert into tblOptions (SLNo, QID, CaptionEng, CaptionBang, Code, QNext ) values ('235','q239_Options', '8.DK','8.Rvwbbv','8','');</v>
       </c>
     </row>

</xml_diff>